<commit_message>
Added handling for cell error codes. Fix of delete drawing bug, thanks Esowers. Some more tests.
</commit_message>
<xml_diff>
--- a/EPPlusTest/Workbooks/FormulaTest.xlsx
+++ b/EPPlusTest/Workbooks/FormulaTest.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="39">
   <si>
     <t>Functions</t>
   </si>
@@ -78,9 +78,6 @@
     <t>Product</t>
   </si>
   <si>
-    <t>Array incl text</t>
-  </si>
-  <si>
     <t>Name Error</t>
   </si>
   <si>
@@ -130,6 +127,27 @@
   </si>
   <si>
     <t>Multi Argument</t>
+  </si>
+  <si>
+    <t>ValueError</t>
+  </si>
+  <si>
+    <t>NA Error</t>
+  </si>
+  <si>
+    <t>Null Error</t>
+  </si>
+  <si>
+    <t>Numerror</t>
+  </si>
+  <si>
+    <t>Array incl text &amp; boolean</t>
+  </si>
+  <si>
+    <t>Errors</t>
+  </si>
+  <si>
+    <t>Div0</t>
   </si>
 </sst>
 </file>
@@ -153,7 +171,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -163,6 +181,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -179,10 +203,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -619,10 +647,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:N27"/>
+  <dimension ref="A1:T27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -636,13 +664,13 @@
     <col min="7" max="7" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.42578125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -650,40 +678,48 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B2">
         <v>3</v>
       </c>
-      <c r="C2" t="e">
-        <f>d</f>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>7</v>
       </c>
-      <c r="C3" t="e">
-        <f>0/0</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B7" t="b">
+        <v>1</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+      <c r="P7" s="3"/>
+      <c r="Q7" s="3"/>
+      <c r="R7" s="3"/>
+      <c r="S7" s="3"/>
+      <c r="T7" s="4"/>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
         <v>2</v>
       </c>
@@ -697,10 +733,10 @@
         <v>4</v>
       </c>
       <c r="F8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G8" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>32</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>7</v>
@@ -709,19 +745,37 @@
         <v>8</v>
       </c>
       <c r="J8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="L8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="L8" s="1" t="s">
+      <c r="M8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="M8" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="N8" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="R8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="S8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="T8" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
@@ -758,23 +812,47 @@
         <v>130</v>
       </c>
       <c r="J9">
-        <f>SUM({1;2;4;"Text"})</f>
+        <f>SUM({1;2;4;"Text";TRUE})</f>
         <v>7</v>
       </c>
       <c r="L9" t="e">
-        <f>SUM(C2)</f>
+        <f>d</f>
         <v>#NAME?</v>
       </c>
       <c r="M9" t="e">
-        <f>SUM(C3)</f>
+        <f>SUM(T9)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="N9" t="e">
+      <c r="N9">
         <f>SUM(C2:C3)</f>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="O9" t="e">
+        <f>1+"a"</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="P9" t="e">
+        <f>VLOOKUP(8,I9:I27,0,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="Q9" t="e">
+        <f>POWER(100,10000000000000)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="R9" t="e">
+        <f>B1 B2</f>
+        <v>#NULL!</v>
+      </c>
+      <c r="S9" t="e">
+        <f>SUM(#REF!:B3)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="T9" t="e">
+        <f>0/0</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -811,11 +889,27 @@
         <v>1</v>
       </c>
       <c r="J10">
-        <f>COUNT({1;2;4;"Text"})</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+        <f>COUNT({1;2;4;"Text";TRUE})</f>
+        <v>3</v>
+      </c>
+      <c r="L10" t="e">
+        <f>SUM(L9)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="O10" t="e">
+        <f>SUBTOTAL(45,J9:J26)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="P10" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="S10" t="e">
+        <f>MAX(#REF!)</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -852,13 +946,25 @@
         <v>1</v>
       </c>
       <c r="J11">
-        <f>COUNTA({1;2;4;"Text"})</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+        <f>COUNTA({1;2;4;"Text";TRUE})</f>
+        <v>5</v>
+      </c>
+      <c r="L11" t="e">
+        <f ca="1">Dp()</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="O11" t="e">
+        <f>SUMPRODUCT(B2,B3:B4)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="S11" t="e">
+        <f>#REF!:#REF!</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B12">
         <f>MIN($B$2)</f>
@@ -893,13 +999,21 @@
         <v>130</v>
       </c>
       <c r="J12">
-        <f>MAX({1;2;4;"Text"})</f>
+        <f>MAX({1;2;4;"Text";TRUE})</f>
         <v>4</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O12" t="e">
+        <f>B1:B2</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="S12" t="e">
+        <f ca="1">D5()</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B13">
         <f>MAX($B$2)</f>
@@ -934,11 +1048,15 @@
         <v>130</v>
       </c>
       <c r="J13">
-        <f>MIN({1;2;4;"Text"})</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+        <f>MIN({1;2;4;"Text";TRUE})</f>
+        <v>1</v>
+      </c>
+      <c r="S13" t="e">
+        <f ca="1">D5(21)</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -975,11 +1093,11 @@
         <v>130</v>
       </c>
       <c r="J14">
-        <f>AVERAGE({1;2;4;"Text"})</f>
+        <f>AVERAGE({1;2;4;"Text";TRUE})</f>
         <v>2.3333333333333335</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -1016,11 +1134,11 @@
         <v>130</v>
       </c>
       <c r="J15">
-        <f>AVERAGEA({1;2;4;"Text"})</f>
+        <f>AVERAGEA({1;2;4;"Text";TRUE})</f>
         <v>1.75</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -1057,13 +1175,13 @@
         <v>130</v>
       </c>
       <c r="J16">
-        <f>PRODUCT({1;2;4;"Text"})</f>
+        <f>PRODUCT({1;2;4;"Text";TRUE})</f>
         <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B17">
         <f>SUBTOTAL(1,B2)</f>
@@ -1095,7 +1213,7 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B18">
         <f>SUBTOTAL(2,$B$2)</f>
@@ -1127,7 +1245,7 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B19">
         <f>SUBTOTAL(3,$B$2)</f>
@@ -1159,7 +1277,7 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B20">
         <f>SUBTOTAL(4,$B$2)</f>
@@ -1191,7 +1309,7 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B21">
         <f>SUBTOTAL(5,$B$2)</f>
@@ -1223,7 +1341,7 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B22">
         <f>SUBTOTAL(6,$B$2)</f>
@@ -1255,7 +1373,7 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B23" t="e">
         <f>SUBTOTAL(7,$B$2)</f>
@@ -1287,7 +1405,7 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B24">
         <f>SUBTOTAL(8,$B$2)</f>
@@ -1319,7 +1437,7 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B25">
         <f>SUBTOTAL(9,$B$2)</f>
@@ -1351,7 +1469,7 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B26" t="e">
         <f>SUBTOTAL(10,$B$2)</f>
@@ -1383,7 +1501,7 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B27">
         <f>SUBTOTAL(11,$B$2)</f>
@@ -1414,6 +1532,9 @@
       <c r="J27" s="2"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="L7:T7"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Added more test cases in Formula Test. Fixed bug in IsEmpty property. Reverted a few files from merge
</commit_message>
<xml_diff>
--- a/EPPlusTest/Workbooks/FormulaTest.xlsx
+++ b/EPPlusTest/Workbooks/FormulaTest.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="41">
   <si>
     <t>Functions</t>
   </si>
@@ -78,9 +78,6 @@
     <t>Product</t>
   </si>
   <si>
-    <t>Array incl text</t>
-  </si>
-  <si>
     <t>Name Error</t>
   </si>
   <si>
@@ -130,6 +127,33 @@
   </si>
   <si>
     <t>Multi Argument</t>
+  </si>
+  <si>
+    <t>ValueError</t>
+  </si>
+  <si>
+    <t>NA Error</t>
+  </si>
+  <si>
+    <t>Null Error</t>
+  </si>
+  <si>
+    <t>Numerror</t>
+  </si>
+  <si>
+    <t>Array incl text &amp; boolean</t>
+  </si>
+  <si>
+    <t>Errors</t>
+  </si>
+  <si>
+    <t>Div0</t>
+  </si>
+  <si>
+    <t>Sum Kolumn</t>
+  </si>
+  <si>
+    <t>Vlookup</t>
   </si>
 </sst>
 </file>
@@ -153,7 +177,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -163,6 +187,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -179,10 +209,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -619,10 +653,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:N27"/>
+  <dimension ref="A1:L41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -636,13 +670,15 @@
     <col min="7" max="7" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.140625" customWidth="1"/>
     <col min="14" max="14" width="11" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -650,7 +686,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B2">
         <v>3</v>
       </c>
@@ -659,7 +695,7 @@
         <v>#NAME?</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>7</v>
       </c>
@@ -668,22 +704,27 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
         <v>2</v>
       </c>
@@ -697,10 +738,10 @@
         <v>4</v>
       </c>
       <c r="F8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G8" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>32</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>7</v>
@@ -709,19 +750,11 @@
         <v>8</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="L8" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="M8" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="N8" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+      <c r="L8" s="1"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
@@ -758,23 +791,15 @@
         <v>130</v>
       </c>
       <c r="J9">
-        <f>SUM({1;2;4;"Text"})</f>
+        <f>SUM({1;2;4;"Text";TRUE})</f>
         <v>7</v>
       </c>
-      <c r="L9" t="e">
-        <f>SUM(C2)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="M9" t="e">
-        <f>SUM(C3)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N9" t="e">
-        <f>SUM(C2:C3)</f>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L9">
+        <f>SUM(4:5)</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -811,11 +836,15 @@
         <v>1</v>
       </c>
       <c r="J10">
-        <f>COUNT({1;2;4;"Text"})</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+        <f>COUNT({1;2;4;"Text";TRUE})</f>
+        <v>3</v>
+      </c>
+      <c r="L10">
+        <f>SUM(5:6)</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -852,13 +881,13 @@
         <v>1</v>
       </c>
       <c r="J11">
-        <f>COUNTA({1;2;4;"Text"})</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+        <f>COUNTA({1;2;4;"Text";TRUE})</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B12">
         <f>MIN($B$2)</f>
@@ -893,13 +922,13 @@
         <v>130</v>
       </c>
       <c r="J12">
-        <f>MAX({1;2;4;"Text"})</f>
+        <f>MAX({1;2;4;"Text";TRUE})</f>
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B13">
         <f>MAX($B$2)</f>
@@ -934,11 +963,11 @@
         <v>130</v>
       </c>
       <c r="J13">
-        <f>MIN({1;2;4;"Text"})</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+        <f>MIN({1;2;4;"Text";TRUE})</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -975,11 +1004,11 @@
         <v>130</v>
       </c>
       <c r="J14">
-        <f>AVERAGE({1;2;4;"Text"})</f>
+        <f>AVERAGE({1;2;4;"Text";TRUE})</f>
         <v>2.3333333333333335</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -1016,11 +1045,11 @@
         <v>130</v>
       </c>
       <c r="J15">
-        <f>AVERAGEA({1;2;4;"Text"})</f>
+        <f>AVERAGEA({1;2;4;"Text";TRUE})</f>
         <v>1.75</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -1057,13 +1086,13 @@
         <v>130</v>
       </c>
       <c r="J16">
-        <f>PRODUCT({1;2;4;"Text"})</f>
+        <f>PRODUCT({1;2;4;"Text";TRUE})</f>
         <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B17">
         <f>SUBTOTAL(1,B2)</f>
@@ -1095,7 +1124,7 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B18">
         <f>SUBTOTAL(2,$B$2)</f>
@@ -1127,7 +1156,7 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B19">
         <f>SUBTOTAL(3,$B$2)</f>
@@ -1159,7 +1188,7 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B20">
         <f>SUBTOTAL(4,$B$2)</f>
@@ -1191,7 +1220,7 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B21">
         <f>SUBTOTAL(5,$B$2)</f>
@@ -1223,7 +1252,7 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B22">
         <f>SUBTOTAL(6,$B$2)</f>
@@ -1255,7 +1284,7 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B23" t="e">
         <f>SUBTOTAL(7,$B$2)</f>
@@ -1287,7 +1316,7 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B24">
         <f>SUBTOTAL(8,$B$2)</f>
@@ -1319,7 +1348,7 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B25">
         <f>SUBTOTAL(9,$B$2)</f>
@@ -1351,7 +1380,7 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B26" t="e">
         <f>SUBTOTAL(10,$B$2)</f>
@@ -1383,7 +1412,7 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B27">
         <f>SUBTOTAL(11,$B$2)</f>
@@ -1413,7 +1442,182 @@
       </c>
       <c r="J27" s="2"/>
     </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B29" t="e">
+        <f>VLOOKUP("7",B2:B6,1)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="C29" t="e">
+        <f>VLOOKUP(8,B2:B6,FALSE)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D29">
+        <f>VLOOKUP(7,B2:B6,1)</f>
+        <v>7</v>
+      </c>
+      <c r="E29" t="e">
+        <f>VLOOKUP(8,{1;2;3;4},1,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F29">
+        <f>VLOOKUP(8,{1;2;3;4;10},1,TRUE)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B31" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B32" t="e">
+        <f>SUM(D:D)</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B33">
+        <f>COUNT(D:D)</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B35" s="3"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="3"/>
+      <c r="H35" s="3"/>
+      <c r="I35" s="4"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" t="e">
+        <f>d</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="B37" t="e">
+        <f>SUM(I37)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C37" t="e">
+        <f>SUM(C2:C3)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="D37" t="e">
+        <f>1+"a"</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E37" t="e">
+        <f>VLOOKUP(8,I9:I27,0,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F37" t="e">
+        <f>POWER(100,10000000000000)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="G37" t="e">
+        <f>B1 B2</f>
+        <v>#NULL!</v>
+      </c>
+      <c r="H37" t="e">
+        <f>SUM(#REF!:B3)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="I37" t="e">
+        <f>0/0</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" t="e">
+        <f>SUM(A37)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="D38" t="e">
+        <f>SUBTOTAL(45,J9:J26)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E38" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H38" t="e">
+        <f>MAX(#REF!)</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" t="e">
+        <f ca="1">Dp()</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="D39" t="e">
+        <f>SUMPRODUCT(B2,B3:B4)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H39" t="e">
+        <f>#REF!:#REF!</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40"/>
+      <c r="D40" t="e">
+        <f>B1:B2</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H40" t="e">
+        <f ca="1">D5()</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41"/>
+      <c r="H41" t="e">
+        <f ca="1">D5(21)</f>
+        <v>#REF!</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A35:I35"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Added some more test scenarios to the test workbook
</commit_message>
<xml_diff>
--- a/EPPlusTest/Workbooks/FormulaTest.xlsx
+++ b/EPPlusTest/Workbooks/FormulaTest.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17835" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17835" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="ValidateFormulas" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="Cells_B2B3">ValidateFormulas!$B$2:$B$3</definedName>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="48">
   <si>
     <t>Functions</t>
   </si>
@@ -154,6 +155,27 @@
   </si>
   <si>
     <t>Vlookup</t>
+  </si>
+  <si>
+    <t>Number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Decimal </t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>FormulaToSum</t>
+  </si>
+  <si>
+    <t>Column1</t>
+  </si>
+  <si>
+    <t>Boolean</t>
   </si>
 </sst>
 </file>
@@ -221,7 +243,11 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -232,6 +258,22 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E30" totalsRowCount="1">
+  <autoFilter ref="A1:E29"/>
+  <tableColumns count="5">
+    <tableColumn id="1" name="Number" totalsRowLabel="Total"/>
+    <tableColumn id="2" name="Decimal " totalsRowFunction="stdDev"/>
+    <tableColumn id="3" name="Test" totalsRowFunction="min"/>
+    <tableColumn id="4" name="FormulaToSum" totalsRowFunction="sum"/>
+    <tableColumn id="5" name="Column1" totalsRowFunction="countNums" dataDxfId="0">
+      <calculatedColumnFormula>Table1[[#This Row],[Test]]+Table1[[#This Row],[FormulaToSum]]*Table1[[#This Row],[Number]]/Table1[[#This Row],[Decimal ]]</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -655,8 +697,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:L41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -794,6 +836,10 @@
         <f>SUM({1;2;4;"Text";TRUE})</f>
         <v>7</v>
       </c>
+      <c r="K9">
+        <f>SUM(Sheet3!E29,Table1[FormulaToSum])+Table1[[#Totals],[Column1]]+Table1[[#Totals],[Decimal ]]</f>
+        <v>2129120.3509751195</v>
+      </c>
       <c r="L9">
         <f>SUM(4:5)</f>
         <v>30</v>
@@ -839,6 +885,10 @@
         <f>COUNT({1;2;4;"Text";TRUE})</f>
         <v>3</v>
       </c>
+      <c r="K10">
+        <f>COUNT(Sheet3!E29,Table1[FormulaToSum])+Table1[[#Totals],[Column1]]+Table1[[#Totals],[Decimal ]]</f>
+        <v>64.225975119502039</v>
+      </c>
       <c r="L10">
         <f>SUM(5:6)</f>
         <v>18</v>
@@ -884,6 +934,10 @@
         <f>COUNTA({1;2;4;"Text";TRUE})</f>
         <v>5</v>
       </c>
+      <c r="K11">
+        <f>COUNTA(Sheet3!E29,Table1[FormulaToSum])+Table1[[#Totals],[Column1]]+Table1[[#Totals],[Decimal ]]</f>
+        <v>64.225975119502039</v>
+      </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
@@ -924,6 +978,10 @@
       <c r="J12">
         <f>MAX({1;2;4;"Text";TRUE})</f>
         <v>4</v>
+      </c>
+      <c r="K12">
+        <f>SUM(Sheet3!E29,Table1[FormulaToSum])+Table1[[#Totals],[Column1]]+Table1[[#Totals],[Decimal ]]</f>
+        <v>2129120.3509751195</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -1471,17 +1529,51 @@
       <c r="B31" s="1" t="s">
         <v>39</v>
       </c>
+      <c r="D31" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B32" t="e">
         <f>SUM(D:D)</f>
         <v>#VALUE!</v>
       </c>
+      <c r="D32" t="b">
+        <f>B4=B3</f>
+        <v>0</v>
+      </c>
+      <c r="E32" t="b">
+        <f>C25=D25</f>
+        <v>1</v>
+      </c>
+      <c r="F32" t="e">
+        <f>E37=E38</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G32" t="b">
+        <f>LEFT(A22,5)=LEFT(A23,5)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B33">
         <f>COUNT(D:D)</f>
         <v>20</v>
+      </c>
+      <c r="D33" t="b">
+        <f>C30=D30</f>
+        <v>1</v>
+      </c>
+      <c r="E33" t="e">
+        <f>D37=D38</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F33" t="e">
+        <f>G37=H37</f>
+        <v>#NULL!</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
@@ -1615,10 +1707,577 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A35:I35"/>
+    <mergeCell ref="D31:G31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.42578125" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>12</v>
+      </c>
+      <c r="B2">
+        <v>3</v>
+      </c>
+      <c r="C2">
+        <v>3</v>
+      </c>
+      <c r="D2">
+        <v>7777</v>
+      </c>
+      <c r="E2">
+        <f>Table1[[#This Row],[Test]]+Table1[[#This Row],[FormulaToSum]]*Table1[[#This Row],[Number]]/Table1[[#This Row],[Decimal ]]</f>
+        <v>31111</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>33</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>99</v>
+      </c>
+      <c r="E3">
+        <f>Table1[[#This Row],[Test]]+Table1[[#This Row],[FormulaToSum]]*Table1[[#This Row],[Number]]/Table1[[#This Row],[Decimal ]]</f>
+        <v>1635.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>54</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>-7579</v>
+      </c>
+      <c r="E4">
+        <f>Table1[[#This Row],[Test]]+Table1[[#This Row],[FormulaToSum]]*Table1[[#This Row],[Number]]/Table1[[#This Row],[Decimal ]]</f>
+        <v>-409265</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>75</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>-15257</v>
+      </c>
+      <c r="E5" t="e">
+        <f>Table1[[#This Row],[Test]]+Table1[[#This Row],[FormulaToSum]]*Table1[[#This Row],[Number]]/Table1[[#This Row],[Decimal ]]</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>96</v>
+      </c>
+      <c r="B6">
+        <v>-1</v>
+      </c>
+      <c r="C6">
+        <v>-1</v>
+      </c>
+      <c r="D6">
+        <v>-22935</v>
+      </c>
+      <c r="E6">
+        <f>Table1[[#This Row],[Test]]+Table1[[#This Row],[FormulaToSum]]*Table1[[#This Row],[Number]]/Table1[[#This Row],[Decimal ]]</f>
+        <v>2201759</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>117</v>
+      </c>
+      <c r="B7">
+        <v>-2</v>
+      </c>
+      <c r="C7">
+        <v>-2</v>
+      </c>
+      <c r="D7">
+        <v>-30613</v>
+      </c>
+      <c r="E7">
+        <f>Table1[[#This Row],[Test]]+Table1[[#This Row],[FormulaToSum]]*Table1[[#This Row],[Number]]/Table1[[#This Row],[Decimal ]]</f>
+        <v>1790858.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>138</v>
+      </c>
+      <c r="B8">
+        <v>-3</v>
+      </c>
+      <c r="C8">
+        <v>-3</v>
+      </c>
+      <c r="D8">
+        <v>-38291</v>
+      </c>
+      <c r="E8">
+        <f>Table1[[#This Row],[Test]]+Table1[[#This Row],[FormulaToSum]]*Table1[[#This Row],[Number]]/Table1[[#This Row],[Decimal ]]</f>
+        <v>1761383</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>159</v>
+      </c>
+      <c r="B9">
+        <v>-4</v>
+      </c>
+      <c r="C9">
+        <v>-4</v>
+      </c>
+      <c r="D9">
+        <v>-45969</v>
+      </c>
+      <c r="E9">
+        <f>Table1[[#This Row],[Test]]+Table1[[#This Row],[FormulaToSum]]*Table1[[#This Row],[Number]]/Table1[[#This Row],[Decimal ]]</f>
+        <v>1827263.75</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>180</v>
+      </c>
+      <c r="B10">
+        <v>-5</v>
+      </c>
+      <c r="C10">
+        <v>-5</v>
+      </c>
+      <c r="D10">
+        <v>-53647</v>
+      </c>
+      <c r="E10">
+        <f>Table1[[#This Row],[Test]]+Table1[[#This Row],[FormulaToSum]]*Table1[[#This Row],[Number]]/Table1[[#This Row],[Decimal ]]</f>
+        <v>1931287</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>201</v>
+      </c>
+      <c r="B11">
+        <v>-6</v>
+      </c>
+      <c r="C11">
+        <v>-6</v>
+      </c>
+      <c r="D11">
+        <v>-61325</v>
+      </c>
+      <c r="E11">
+        <f>Table1[[#This Row],[Test]]+Table1[[#This Row],[FormulaToSum]]*Table1[[#This Row],[Number]]/Table1[[#This Row],[Decimal ]]</f>
+        <v>2054381.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>222</v>
+      </c>
+      <c r="B12">
+        <v>-7</v>
+      </c>
+      <c r="C12">
+        <v>-7</v>
+      </c>
+      <c r="D12">
+        <v>-69003</v>
+      </c>
+      <c r="E12">
+        <f>Table1[[#This Row],[Test]]+Table1[[#This Row],[FormulaToSum]]*Table1[[#This Row],[Number]]/Table1[[#This Row],[Decimal ]]</f>
+        <v>2188373.8571428573</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>243</v>
+      </c>
+      <c r="B13">
+        <v>-8</v>
+      </c>
+      <c r="C13">
+        <v>-8</v>
+      </c>
+      <c r="D13">
+        <v>-76681</v>
+      </c>
+      <c r="E13">
+        <f>Table1[[#This Row],[Test]]+Table1[[#This Row],[FormulaToSum]]*Table1[[#This Row],[Number]]/Table1[[#This Row],[Decimal ]]</f>
+        <v>2329177.375</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>264</v>
+      </c>
+      <c r="B14">
+        <v>-9</v>
+      </c>
+      <c r="C14">
+        <v>-9</v>
+      </c>
+      <c r="D14">
+        <v>-84359</v>
+      </c>
+      <c r="E14">
+        <f>Table1[[#This Row],[Test]]+Table1[[#This Row],[FormulaToSum]]*Table1[[#This Row],[Number]]/Table1[[#This Row],[Decimal ]]</f>
+        <v>2474521.6666666665</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>285</v>
+      </c>
+      <c r="B15">
+        <v>-10</v>
+      </c>
+      <c r="C15">
+        <v>-10</v>
+      </c>
+      <c r="D15">
+        <v>-92037</v>
+      </c>
+      <c r="E15">
+        <f>Table1[[#This Row],[Test]]+Table1[[#This Row],[FormulaToSum]]*Table1[[#This Row],[Number]]/Table1[[#This Row],[Decimal ]]</f>
+        <v>2623044.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>306</v>
+      </c>
+      <c r="B16">
+        <v>-11</v>
+      </c>
+      <c r="C16">
+        <v>-11</v>
+      </c>
+      <c r="D16">
+        <v>-99715</v>
+      </c>
+      <c r="E16">
+        <f>Table1[[#This Row],[Test]]+Table1[[#This Row],[FormulaToSum]]*Table1[[#This Row],[Number]]/Table1[[#This Row],[Decimal ]]</f>
+        <v>2773879</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>327</v>
+      </c>
+      <c r="B17">
+        <v>-12</v>
+      </c>
+      <c r="C17">
+        <v>-12</v>
+      </c>
+      <c r="D17">
+        <v>-107393</v>
+      </c>
+      <c r="E17">
+        <f>Table1[[#This Row],[Test]]+Table1[[#This Row],[FormulaToSum]]*Table1[[#This Row],[Number]]/Table1[[#This Row],[Decimal ]]</f>
+        <v>2926447.25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>348</v>
+      </c>
+      <c r="B18">
+        <v>-13</v>
+      </c>
+      <c r="C18">
+        <v>-13</v>
+      </c>
+      <c r="D18">
+        <v>-115071</v>
+      </c>
+      <c r="E18">
+        <f>Table1[[#This Row],[Test]]+Table1[[#This Row],[FormulaToSum]]*Table1[[#This Row],[Number]]/Table1[[#This Row],[Decimal ]]</f>
+        <v>3080349.153846154</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>369</v>
+      </c>
+      <c r="B19">
+        <v>-14</v>
+      </c>
+      <c r="C19">
+        <v>-14</v>
+      </c>
+      <c r="D19">
+        <v>-122749</v>
+      </c>
+      <c r="E19">
+        <f>Table1[[#This Row],[Test]]+Table1[[#This Row],[FormulaToSum]]*Table1[[#This Row],[Number]]/Table1[[#This Row],[Decimal ]]</f>
+        <v>3235298.9285714286</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>390</v>
+      </c>
+      <c r="B20">
+        <v>-15</v>
+      </c>
+      <c r="C20">
+        <v>-15</v>
+      </c>
+      <c r="D20">
+        <v>-130427</v>
+      </c>
+      <c r="E20">
+        <f>Table1[[#This Row],[Test]]+Table1[[#This Row],[FormulaToSum]]*Table1[[#This Row],[Number]]/Table1[[#This Row],[Decimal ]]</f>
+        <v>3391087</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>411</v>
+      </c>
+      <c r="B21">
+        <v>-16</v>
+      </c>
+      <c r="C21">
+        <v>-16</v>
+      </c>
+      <c r="D21">
+        <v>-138105</v>
+      </c>
+      <c r="E21">
+        <f>Table1[[#This Row],[Test]]+Table1[[#This Row],[FormulaToSum]]*Table1[[#This Row],[Number]]/Table1[[#This Row],[Decimal ]]</f>
+        <v>3547556.1875</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>432</v>
+      </c>
+      <c r="B22">
+        <v>-17</v>
+      </c>
+      <c r="C22">
+        <v>-17</v>
+      </c>
+      <c r="D22">
+        <v>-145783</v>
+      </c>
+      <c r="E22">
+        <f>Table1[[#This Row],[Test]]+Table1[[#This Row],[FormulaToSum]]*Table1[[#This Row],[Number]]/Table1[[#This Row],[Decimal ]]</f>
+        <v>3704586.2941176472</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>453</v>
+      </c>
+      <c r="B23">
+        <v>-18</v>
+      </c>
+      <c r="C23">
+        <v>-18</v>
+      </c>
+      <c r="D23">
+        <v>-153461</v>
+      </c>
+      <c r="E23">
+        <f>Table1[[#This Row],[Test]]+Table1[[#This Row],[FormulaToSum]]*Table1[[#This Row],[Number]]/Table1[[#This Row],[Decimal ]]</f>
+        <v>3862083.8333333335</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>474</v>
+      </c>
+      <c r="B24">
+        <v>-19</v>
+      </c>
+      <c r="C24">
+        <v>-19</v>
+      </c>
+      <c r="D24">
+        <v>-161139</v>
+      </c>
+      <c r="E24">
+        <f>Table1[[#This Row],[Test]]+Table1[[#This Row],[FormulaToSum]]*Table1[[#This Row],[Number]]/Table1[[#This Row],[Decimal ]]</f>
+        <v>4019975</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>495</v>
+      </c>
+      <c r="B25">
+        <v>-20</v>
+      </c>
+      <c r="C25">
+        <v>-20</v>
+      </c>
+      <c r="D25">
+        <v>-168817</v>
+      </c>
+      <c r="E25">
+        <f>Table1[[#This Row],[Test]]+Table1[[#This Row],[FormulaToSum]]*Table1[[#This Row],[Number]]/Table1[[#This Row],[Decimal ]]</f>
+        <v>4178200.75</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>516</v>
+      </c>
+      <c r="B26">
+        <v>-21</v>
+      </c>
+      <c r="C26">
+        <v>-21</v>
+      </c>
+      <c r="D26">
+        <v>-176495</v>
+      </c>
+      <c r="E26">
+        <f>Table1[[#This Row],[Test]]+Table1[[#This Row],[FormulaToSum]]*Table1[[#This Row],[Number]]/Table1[[#This Row],[Decimal ]]</f>
+        <v>4336713.2857142854</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>537</v>
+      </c>
+      <c r="B27">
+        <v>-22</v>
+      </c>
+      <c r="C27">
+        <v>-22</v>
+      </c>
+      <c r="D27">
+        <v>-184173</v>
+      </c>
+      <c r="E27">
+        <f>Table1[[#This Row],[Test]]+Table1[[#This Row],[FormulaToSum]]*Table1[[#This Row],[Number]]/Table1[[#This Row],[Decimal ]]</f>
+        <v>4495473.5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>558</v>
+      </c>
+      <c r="B28">
+        <v>-23</v>
+      </c>
+      <c r="C28">
+        <v>-23</v>
+      </c>
+      <c r="D28">
+        <v>-191851</v>
+      </c>
+      <c r="E28">
+        <f>Table1[[#This Row],[Test]]+Table1[[#This Row],[FormulaToSum]]*Table1[[#This Row],[Number]]/Table1[[#This Row],[Decimal ]]</f>
+        <v>4654449.0869565215</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>579</v>
+      </c>
+      <c r="B29">
+        <v>-24</v>
+      </c>
+      <c r="C29">
+        <v>-24</v>
+      </c>
+      <c r="D29">
+        <v>-199529</v>
+      </c>
+      <c r="E29">
+        <f>Table1[[#This Row],[Test]]+Table1[[#This Row],[FormulaToSum]]*Table1[[#This Row],[Number]]/Table1[[#This Row],[Decimal ]]</f>
+        <v>4813613.125</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>44</v>
+      </c>
+      <c r="B30">
+        <f>SUBTOTAL(107,Table1[[Decimal ]])</f>
+        <v>8.2259751195020439</v>
+      </c>
+      <c r="C30">
+        <f>SUBTOTAL(105,Table1[Test])</f>
+        <v>-24</v>
+      </c>
+      <c r="D30">
+        <f>SUBTOTAL(109,Table1[FormulaToSum])</f>
+        <v>-2684528</v>
+      </c>
+      <c r="E30">
+        <f>SUBTOTAL(102,Table1[Column1])</f>
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Merged with Jans changes of FormulaTest.xlsx
</commit_message>
<xml_diff>
--- a/EPPlusTest/Workbooks/FormulaTest.xlsx
+++ b/EPPlusTest/Workbooks/FormulaTest.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17835" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17835" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="ValidateFormulas" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="Cells_B2B3">ValidateFormulas!$B$2:$B$3</definedName>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="48">
   <si>
     <t>Functions</t>
   </si>
@@ -154,6 +155,27 @@
   </si>
   <si>
     <t>Vlookup</t>
+  </si>
+  <si>
+    <t>Number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Decimal </t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>FormulaToSum</t>
+  </si>
+  <si>
+    <t>Column1</t>
+  </si>
+  <si>
+    <t>Boolean</t>
   </si>
 </sst>
 </file>
@@ -221,7 +243,11 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -232,6 +258,22 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E30" totalsRowCount="1">
+  <autoFilter ref="A1:E29"/>
+  <tableColumns count="5">
+    <tableColumn id="1" name="Number" totalsRowLabel="Total"/>
+    <tableColumn id="2" name="Decimal " totalsRowFunction="stdDev"/>
+    <tableColumn id="3" name="Test" totalsRowFunction="min"/>
+    <tableColumn id="4" name="FormulaToSum" totalsRowFunction="sum"/>
+    <tableColumn id="5" name="Column1" totalsRowFunction="countNums" dataDxfId="0">
+      <calculatedColumnFormula>Table1[[#This Row],[Test]]+Table1[[#This Row],[FormulaToSum]]*Table1[[#This Row],[Number]]/Table1[[#This Row],[Decimal ]]</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -655,8 +697,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:L41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -794,6 +836,10 @@
         <f>SUM({1;2;4;"Text";TRUE})</f>
         <v>7</v>
       </c>
+      <c r="K9">
+        <f>SUM(Sheet3!E29,Table1[FormulaToSum])+Table1[[#Totals],[Column1]]+Table1[[#Totals],[Decimal ]]</f>
+        <v>2129120.3509751195</v>
+      </c>
       <c r="L9">
         <f>SUM(4:5)</f>
         <v>30</v>
@@ -839,6 +885,10 @@
         <f>COUNT({1;2;4;"Text";TRUE})</f>
         <v>3</v>
       </c>
+      <c r="K10">
+        <f>COUNT(Sheet3!E29,Table1[FormulaToSum])+Table1[[#Totals],[Column1]]+Table1[[#Totals],[Decimal ]]</f>
+        <v>64.225975119502039</v>
+      </c>
       <c r="L10">
         <f>SUM(5:6)</f>
         <v>18</v>
@@ -884,6 +934,10 @@
         <f>COUNTA({1;2;4;"Text";TRUE})</f>
         <v>5</v>
       </c>
+      <c r="K11">
+        <f>COUNTA(Sheet3!E29,Table1[FormulaToSum])+Table1[[#Totals],[Column1]]+Table1[[#Totals],[Decimal ]]</f>
+        <v>64.225975119502039</v>
+      </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
@@ -924,6 +978,10 @@
       <c r="J12">
         <f>MAX({1;2;4;"Text";TRUE})</f>
         <v>4</v>
+      </c>
+      <c r="K12">
+        <f>SUM(Sheet3!E29,Table1[FormulaToSum])+Table1[[#Totals],[Column1]]+Table1[[#Totals],[Decimal ]]</f>
+        <v>2129120.3509751195</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -1471,17 +1529,51 @@
       <c r="B31" s="1" t="s">
         <v>39</v>
       </c>
+      <c r="D31" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B32" t="e">
         <f>SUM(D:D)</f>
         <v>#VALUE!</v>
       </c>
+      <c r="D32" t="b">
+        <f>B4=B3</f>
+        <v>0</v>
+      </c>
+      <c r="E32" t="b">
+        <f>C25=D25</f>
+        <v>1</v>
+      </c>
+      <c r="F32" t="e">
+        <f>E37=E38</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G32" t="b">
+        <f>LEFT(A22,5)=LEFT(A23,5)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B33">
         <f>COUNT(D:D)</f>
         <v>20</v>
+      </c>
+      <c r="D33" t="b">
+        <f>C30=D30</f>
+        <v>1</v>
+      </c>
+      <c r="E33" t="e">
+        <f>D37=D38</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F33" t="e">
+        <f>G37=H37</f>
+        <v>#NULL!</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
@@ -1615,10 +1707,577 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A35:I35"/>
+    <mergeCell ref="D31:G31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.42578125" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>12</v>
+      </c>
+      <c r="B2">
+        <v>3</v>
+      </c>
+      <c r="C2">
+        <v>3</v>
+      </c>
+      <c r="D2">
+        <v>7777</v>
+      </c>
+      <c r="E2">
+        <f>Table1[[#This Row],[Test]]+Table1[[#This Row],[FormulaToSum]]*Table1[[#This Row],[Number]]/Table1[[#This Row],[Decimal ]]</f>
+        <v>31111</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>33</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>99</v>
+      </c>
+      <c r="E3">
+        <f>Table1[[#This Row],[Test]]+Table1[[#This Row],[FormulaToSum]]*Table1[[#This Row],[Number]]/Table1[[#This Row],[Decimal ]]</f>
+        <v>1635.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>54</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>-7579</v>
+      </c>
+      <c r="E4">
+        <f>Table1[[#This Row],[Test]]+Table1[[#This Row],[FormulaToSum]]*Table1[[#This Row],[Number]]/Table1[[#This Row],[Decimal ]]</f>
+        <v>-409265</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>75</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>-15257</v>
+      </c>
+      <c r="E5" t="e">
+        <f>Table1[[#This Row],[Test]]+Table1[[#This Row],[FormulaToSum]]*Table1[[#This Row],[Number]]/Table1[[#This Row],[Decimal ]]</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>96</v>
+      </c>
+      <c r="B6">
+        <v>-1</v>
+      </c>
+      <c r="C6">
+        <v>-1</v>
+      </c>
+      <c r="D6">
+        <v>-22935</v>
+      </c>
+      <c r="E6">
+        <f>Table1[[#This Row],[Test]]+Table1[[#This Row],[FormulaToSum]]*Table1[[#This Row],[Number]]/Table1[[#This Row],[Decimal ]]</f>
+        <v>2201759</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>117</v>
+      </c>
+      <c r="B7">
+        <v>-2</v>
+      </c>
+      <c r="C7">
+        <v>-2</v>
+      </c>
+      <c r="D7">
+        <v>-30613</v>
+      </c>
+      <c r="E7">
+        <f>Table1[[#This Row],[Test]]+Table1[[#This Row],[FormulaToSum]]*Table1[[#This Row],[Number]]/Table1[[#This Row],[Decimal ]]</f>
+        <v>1790858.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>138</v>
+      </c>
+      <c r="B8">
+        <v>-3</v>
+      </c>
+      <c r="C8">
+        <v>-3</v>
+      </c>
+      <c r="D8">
+        <v>-38291</v>
+      </c>
+      <c r="E8">
+        <f>Table1[[#This Row],[Test]]+Table1[[#This Row],[FormulaToSum]]*Table1[[#This Row],[Number]]/Table1[[#This Row],[Decimal ]]</f>
+        <v>1761383</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>159</v>
+      </c>
+      <c r="B9">
+        <v>-4</v>
+      </c>
+      <c r="C9">
+        <v>-4</v>
+      </c>
+      <c r="D9">
+        <v>-45969</v>
+      </c>
+      <c r="E9">
+        <f>Table1[[#This Row],[Test]]+Table1[[#This Row],[FormulaToSum]]*Table1[[#This Row],[Number]]/Table1[[#This Row],[Decimal ]]</f>
+        <v>1827263.75</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>180</v>
+      </c>
+      <c r="B10">
+        <v>-5</v>
+      </c>
+      <c r="C10">
+        <v>-5</v>
+      </c>
+      <c r="D10">
+        <v>-53647</v>
+      </c>
+      <c r="E10">
+        <f>Table1[[#This Row],[Test]]+Table1[[#This Row],[FormulaToSum]]*Table1[[#This Row],[Number]]/Table1[[#This Row],[Decimal ]]</f>
+        <v>1931287</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>201</v>
+      </c>
+      <c r="B11">
+        <v>-6</v>
+      </c>
+      <c r="C11">
+        <v>-6</v>
+      </c>
+      <c r="D11">
+        <v>-61325</v>
+      </c>
+      <c r="E11">
+        <f>Table1[[#This Row],[Test]]+Table1[[#This Row],[FormulaToSum]]*Table1[[#This Row],[Number]]/Table1[[#This Row],[Decimal ]]</f>
+        <v>2054381.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>222</v>
+      </c>
+      <c r="B12">
+        <v>-7</v>
+      </c>
+      <c r="C12">
+        <v>-7</v>
+      </c>
+      <c r="D12">
+        <v>-69003</v>
+      </c>
+      <c r="E12">
+        <f>Table1[[#This Row],[Test]]+Table1[[#This Row],[FormulaToSum]]*Table1[[#This Row],[Number]]/Table1[[#This Row],[Decimal ]]</f>
+        <v>2188373.8571428573</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>243</v>
+      </c>
+      <c r="B13">
+        <v>-8</v>
+      </c>
+      <c r="C13">
+        <v>-8</v>
+      </c>
+      <c r="D13">
+        <v>-76681</v>
+      </c>
+      <c r="E13">
+        <f>Table1[[#This Row],[Test]]+Table1[[#This Row],[FormulaToSum]]*Table1[[#This Row],[Number]]/Table1[[#This Row],[Decimal ]]</f>
+        <v>2329177.375</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>264</v>
+      </c>
+      <c r="B14">
+        <v>-9</v>
+      </c>
+      <c r="C14">
+        <v>-9</v>
+      </c>
+      <c r="D14">
+        <v>-84359</v>
+      </c>
+      <c r="E14">
+        <f>Table1[[#This Row],[Test]]+Table1[[#This Row],[FormulaToSum]]*Table1[[#This Row],[Number]]/Table1[[#This Row],[Decimal ]]</f>
+        <v>2474521.6666666665</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>285</v>
+      </c>
+      <c r="B15">
+        <v>-10</v>
+      </c>
+      <c r="C15">
+        <v>-10</v>
+      </c>
+      <c r="D15">
+        <v>-92037</v>
+      </c>
+      <c r="E15">
+        <f>Table1[[#This Row],[Test]]+Table1[[#This Row],[FormulaToSum]]*Table1[[#This Row],[Number]]/Table1[[#This Row],[Decimal ]]</f>
+        <v>2623044.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>306</v>
+      </c>
+      <c r="B16">
+        <v>-11</v>
+      </c>
+      <c r="C16">
+        <v>-11</v>
+      </c>
+      <c r="D16">
+        <v>-99715</v>
+      </c>
+      <c r="E16">
+        <f>Table1[[#This Row],[Test]]+Table1[[#This Row],[FormulaToSum]]*Table1[[#This Row],[Number]]/Table1[[#This Row],[Decimal ]]</f>
+        <v>2773879</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>327</v>
+      </c>
+      <c r="B17">
+        <v>-12</v>
+      </c>
+      <c r="C17">
+        <v>-12</v>
+      </c>
+      <c r="D17">
+        <v>-107393</v>
+      </c>
+      <c r="E17">
+        <f>Table1[[#This Row],[Test]]+Table1[[#This Row],[FormulaToSum]]*Table1[[#This Row],[Number]]/Table1[[#This Row],[Decimal ]]</f>
+        <v>2926447.25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>348</v>
+      </c>
+      <c r="B18">
+        <v>-13</v>
+      </c>
+      <c r="C18">
+        <v>-13</v>
+      </c>
+      <c r="D18">
+        <v>-115071</v>
+      </c>
+      <c r="E18">
+        <f>Table1[[#This Row],[Test]]+Table1[[#This Row],[FormulaToSum]]*Table1[[#This Row],[Number]]/Table1[[#This Row],[Decimal ]]</f>
+        <v>3080349.153846154</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>369</v>
+      </c>
+      <c r="B19">
+        <v>-14</v>
+      </c>
+      <c r="C19">
+        <v>-14</v>
+      </c>
+      <c r="D19">
+        <v>-122749</v>
+      </c>
+      <c r="E19">
+        <f>Table1[[#This Row],[Test]]+Table1[[#This Row],[FormulaToSum]]*Table1[[#This Row],[Number]]/Table1[[#This Row],[Decimal ]]</f>
+        <v>3235298.9285714286</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>390</v>
+      </c>
+      <c r="B20">
+        <v>-15</v>
+      </c>
+      <c r="C20">
+        <v>-15</v>
+      </c>
+      <c r="D20">
+        <v>-130427</v>
+      </c>
+      <c r="E20">
+        <f>Table1[[#This Row],[Test]]+Table1[[#This Row],[FormulaToSum]]*Table1[[#This Row],[Number]]/Table1[[#This Row],[Decimal ]]</f>
+        <v>3391087</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>411</v>
+      </c>
+      <c r="B21">
+        <v>-16</v>
+      </c>
+      <c r="C21">
+        <v>-16</v>
+      </c>
+      <c r="D21">
+        <v>-138105</v>
+      </c>
+      <c r="E21">
+        <f>Table1[[#This Row],[Test]]+Table1[[#This Row],[FormulaToSum]]*Table1[[#This Row],[Number]]/Table1[[#This Row],[Decimal ]]</f>
+        <v>3547556.1875</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>432</v>
+      </c>
+      <c r="B22">
+        <v>-17</v>
+      </c>
+      <c r="C22">
+        <v>-17</v>
+      </c>
+      <c r="D22">
+        <v>-145783</v>
+      </c>
+      <c r="E22">
+        <f>Table1[[#This Row],[Test]]+Table1[[#This Row],[FormulaToSum]]*Table1[[#This Row],[Number]]/Table1[[#This Row],[Decimal ]]</f>
+        <v>3704586.2941176472</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>453</v>
+      </c>
+      <c r="B23">
+        <v>-18</v>
+      </c>
+      <c r="C23">
+        <v>-18</v>
+      </c>
+      <c r="D23">
+        <v>-153461</v>
+      </c>
+      <c r="E23">
+        <f>Table1[[#This Row],[Test]]+Table1[[#This Row],[FormulaToSum]]*Table1[[#This Row],[Number]]/Table1[[#This Row],[Decimal ]]</f>
+        <v>3862083.8333333335</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>474</v>
+      </c>
+      <c r="B24">
+        <v>-19</v>
+      </c>
+      <c r="C24">
+        <v>-19</v>
+      </c>
+      <c r="D24">
+        <v>-161139</v>
+      </c>
+      <c r="E24">
+        <f>Table1[[#This Row],[Test]]+Table1[[#This Row],[FormulaToSum]]*Table1[[#This Row],[Number]]/Table1[[#This Row],[Decimal ]]</f>
+        <v>4019975</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>495</v>
+      </c>
+      <c r="B25">
+        <v>-20</v>
+      </c>
+      <c r="C25">
+        <v>-20</v>
+      </c>
+      <c r="D25">
+        <v>-168817</v>
+      </c>
+      <c r="E25">
+        <f>Table1[[#This Row],[Test]]+Table1[[#This Row],[FormulaToSum]]*Table1[[#This Row],[Number]]/Table1[[#This Row],[Decimal ]]</f>
+        <v>4178200.75</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>516</v>
+      </c>
+      <c r="B26">
+        <v>-21</v>
+      </c>
+      <c r="C26">
+        <v>-21</v>
+      </c>
+      <c r="D26">
+        <v>-176495</v>
+      </c>
+      <c r="E26">
+        <f>Table1[[#This Row],[Test]]+Table1[[#This Row],[FormulaToSum]]*Table1[[#This Row],[Number]]/Table1[[#This Row],[Decimal ]]</f>
+        <v>4336713.2857142854</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>537</v>
+      </c>
+      <c r="B27">
+        <v>-22</v>
+      </c>
+      <c r="C27">
+        <v>-22</v>
+      </c>
+      <c r="D27">
+        <v>-184173</v>
+      </c>
+      <c r="E27">
+        <f>Table1[[#This Row],[Test]]+Table1[[#This Row],[FormulaToSum]]*Table1[[#This Row],[Number]]/Table1[[#This Row],[Decimal ]]</f>
+        <v>4495473.5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>558</v>
+      </c>
+      <c r="B28">
+        <v>-23</v>
+      </c>
+      <c r="C28">
+        <v>-23</v>
+      </c>
+      <c r="D28">
+        <v>-191851</v>
+      </c>
+      <c r="E28">
+        <f>Table1[[#This Row],[Test]]+Table1[[#This Row],[FormulaToSum]]*Table1[[#This Row],[Number]]/Table1[[#This Row],[Decimal ]]</f>
+        <v>4654449.0869565215</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>579</v>
+      </c>
+      <c r="B29">
+        <v>-24</v>
+      </c>
+      <c r="C29">
+        <v>-24</v>
+      </c>
+      <c r="D29">
+        <v>-199529</v>
+      </c>
+      <c r="E29">
+        <f>Table1[[#This Row],[Test]]+Table1[[#This Row],[FormulaToSum]]*Table1[[#This Row],[Number]]/Table1[[#This Row],[Decimal ]]</f>
+        <v>4813613.125</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>44</v>
+      </c>
+      <c r="B30">
+        <f>SUBTOTAL(107,Table1[[Decimal ]])</f>
+        <v>8.2259751195020439</v>
+      </c>
+      <c r="C30">
+        <f>SUBTOTAL(105,Table1[Test])</f>
+        <v>-24</v>
+      </c>
+      <c r="D30">
+        <f>SUBTOTAL(109,Table1[FormulaToSum])</f>
+        <v>-2684528</v>
+      </c>
+      <c r="E30">
+        <f>SUBTOTAL(102,Table1[Column1])</f>
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed invalid worksheet name handling in dependency chains. Bug in Merge with functions.
</commit_message>
<xml_diff>
--- a/EPPlusTest/Workbooks/FormulaTest.xlsx
+++ b/EPPlusTest/Workbooks/FormulaTest.xlsx
@@ -268,7 +268,7 @@
     <tableColumn id="2" name="Decimal " totalsRowFunction="stdDev"/>
     <tableColumn id="3" name="Test" totalsRowFunction="min"/>
     <tableColumn id="4" name="FormulaToSum" totalsRowFunction="sum"/>
-    <tableColumn id="5" name="Column1" totalsRowFunction="countNums" dataDxfId="0">
+    <tableColumn id="5" name="Column1" totalsRowFunction="count" dataDxfId="0">
       <calculatedColumnFormula>Table1[[#This Row],[Test]]+Table1[[#This Row],[FormulaToSum]]*Table1[[#This Row],[Number]]/Table1[[#This Row],[Decimal ]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -698,7 +698,7 @@
   <dimension ref="A1:L41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -729,6 +729,10 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <f>Sheet2!A1+B9+Sheet2!A9+J9</f>
+        <v>16</v>
+      </c>
       <c r="B2">
         <v>3</v>
       </c>
@@ -838,7 +842,7 @@
       </c>
       <c r="K9">
         <f>SUM(Sheet3!E29,Table1[FormulaToSum])+Table1[[#Totals],[Column1]]+Table1[[#Totals],[Decimal ]]</f>
-        <v>2129120.3509751195</v>
+        <v>2129121.3509751195</v>
       </c>
       <c r="L9">
         <f>SUM(4:5)</f>
@@ -887,7 +891,7 @@
       </c>
       <c r="K10">
         <f>COUNT(Sheet3!E29,Table1[FormulaToSum])+Table1[[#Totals],[Column1]]+Table1[[#Totals],[Decimal ]]</f>
-        <v>64.225975119502039</v>
+        <v>65.225975119502039</v>
       </c>
       <c r="L10">
         <f>SUM(5:6)</f>
@@ -936,7 +940,7 @@
       </c>
       <c r="K11">
         <f>COUNTA(Sheet3!E29,Table1[FormulaToSum])+Table1[[#Totals],[Column1]]+Table1[[#Totals],[Decimal ]]</f>
-        <v>64.225975119502039</v>
+        <v>65.225975119502039</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -981,7 +985,7 @@
       </c>
       <c r="K12">
         <f>SUM(Sheet3!E29,Table1[FormulaToSum])+Table1[[#Totals],[Column1]]+Table1[[#Totals],[Decimal ]]</f>
-        <v>2129120.3509751195</v>
+        <v>2129121.3509751195</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -1721,7 +1725,7 @@
   <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2270,8 +2274,8 @@
         <v>-2684528</v>
       </c>
       <c r="E30">
-        <f>SUBTOTAL(102,Table1[Column1])</f>
-        <v>27</v>
+        <f>SUBTOTAL(103,Table1[Column1])</f>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed tests failing due to floating point precision
</commit_message>
<xml_diff>
--- a/EPPlusTest/Workbooks/FormulaTest.xlsx
+++ b/EPPlusTest/Workbooks/FormulaTest.xlsx
@@ -20,6 +20,7 @@
   <definedNames>
     <definedName name="Cells_B2B3">ValidateFormulas!$B$2:$B$3</definedName>
     <definedName name="Name">Sheet1!$C$1</definedName>
+    <definedName name="Name_G5">Sheet3!$G$5</definedName>
     <definedName name="NameName">Name+Sheet1!$D$5</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
@@ -698,7 +699,7 @@
   <dimension ref="A1:L41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1722,10 +1723,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N21" sqref="N21"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1736,7 +1737,7 @@
     <col min="5" max="5" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>41</v>
       </c>
@@ -1753,7 +1754,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>12</v>
       </c>
@@ -1771,7 +1772,7 @@
         <v>31111</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>33</v>
       </c>
@@ -1788,8 +1789,12 @@
         <f>Table1[[#This Row],[Test]]+Table1[[#This Row],[FormulaToSum]]*Table1[[#This Row],[Number]]/Table1[[#This Row],[Decimal ]]</f>
         <v>1635.5</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G3" t="e">
+        <f>B32+Sheet1!A3</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>54</v>
       </c>
@@ -1807,7 +1812,7 @@
         <v>-409265</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>75</v>
       </c>
@@ -1824,8 +1829,12 @@
         <f>Table1[[#This Row],[Test]]+Table1[[#This Row],[FormulaToSum]]*Table1[[#This Row],[Number]]/Table1[[#This Row],[Decimal ]]</f>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G5" t="e">
+        <f>Table1[[#This Row],[Column1]]+1</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>96</v>
       </c>
@@ -1843,7 +1852,7 @@
         <v>2201759</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>117</v>
       </c>
@@ -1861,7 +1870,7 @@
         <v>1790858.5</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>138</v>
       </c>
@@ -1879,7 +1888,7 @@
         <v>1761383</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>159</v>
       </c>
@@ -1897,7 +1906,7 @@
         <v>1827263.75</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>180</v>
       </c>
@@ -1915,7 +1924,7 @@
         <v>1931287</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>201</v>
       </c>
@@ -1933,7 +1942,7 @@
         <v>2054381.5</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>222</v>
       </c>
@@ -1951,7 +1960,7 @@
         <v>2188373.8571428573</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>243</v>
       </c>
@@ -1969,7 +1978,7 @@
         <v>2329177.375</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>264</v>
       </c>
@@ -1987,7 +1996,7 @@
         <v>2474521.6666666665</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>285</v>
       </c>
@@ -2005,7 +2014,7 @@
         <v>2623044.5</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>306</v>
       </c>
@@ -2276,6 +2285,12 @@
       <c r="E30">
         <f>SUBTOTAL(103,Table1[Column1])</f>
         <v>28</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B32" t="e">
+        <f>Name_G5+A9</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed error with table addresses. Added new test in test sheet.
</commit_message>
<xml_diff>
--- a/EPPlusTest/Workbooks/FormulaTest.xlsx
+++ b/EPPlusTest/Workbooks/FormulaTest.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17835" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17835" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -200,7 +200,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -219,6 +219,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -232,7 +238,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -240,6 +246,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="10" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -696,10 +705,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:L41"/>
+  <dimension ref="A1:P41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P3" sqref="P3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -721,15 +730,19 @@
     <col min="16" max="16" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C1">
+        <f>((L3-I3)/I3)/P3</f>
+        <v>-18.034296710838554</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <f>Sheet2!A1+B9+Sheet2!A9+J9</f>
         <v>16</v>
@@ -742,7 +755,7 @@
         <v>#NAME?</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>7</v>
       </c>
@@ -750,28 +763,37 @@
         <f>0/0</f>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I3">
+        <v>349578723238.39771</v>
+      </c>
+      <c r="L3">
+        <v>409371020621.32922</v>
+      </c>
+      <c r="P3" s="5">
+        <v>-9.4842073007525979E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B7" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
         <v>2</v>
       </c>
@@ -801,7 +823,7 @@
       </c>
       <c r="L8" s="1"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
@@ -850,7 +872,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -899,7 +921,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -944,7 +966,7 @@
         <v>65.225975119502039</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>29</v>
       </c>
@@ -989,7 +1011,7 @@
         <v>2129121.3509751195</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>28</v>
       </c>
@@ -1030,7 +1052,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -1071,7 +1093,7 @@
         <v>2.3333333333333335</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -1112,7 +1134,7 @@
         <v>1.75</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -1723,9 +1745,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fixed a few bugs in the dependency chain handler. Added some new tests.
</commit_message>
<xml_diff>
--- a/EPPlusTest/Workbooks/FormulaTest.xlsx
+++ b/EPPlusTest/Workbooks/FormulaTest.xlsx
@@ -242,13 +242,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="10" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -708,7 +708,7 @@
   <dimension ref="A1:P41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P3" sqref="P3"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -741,6 +741,10 @@
         <f>((L3-I3)/I3)/P3</f>
         <v>-18.034296710838554</v>
       </c>
+      <c r="D1">
+        <f>A2+-1</f>
+        <v>15</v>
+      </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
@@ -754,6 +758,10 @@
         <f>d</f>
         <v>#NAME?</v>
       </c>
+      <c r="D2">
+        <f>A2*-1</f>
+        <v>-16</v>
+      </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B3">
@@ -763,13 +771,17 @@
         <f>0/0</f>
         <v>#DIV/0!</v>
       </c>
+      <c r="D3">
+        <f>D1*1</f>
+        <v>15</v>
+      </c>
       <c r="I3">
         <v>349578723238.39771</v>
       </c>
       <c r="L3">
         <v>409371020621.32922</v>
       </c>
-      <c r="P3" s="5">
+      <c r="P3" s="3">
         <v>-9.4842073007525979E-3</v>
       </c>
     </row>
@@ -1556,12 +1568,12 @@
       <c r="B31" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D31" s="3" t="s">
+      <c r="D31" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="E31" s="3"/>
-      <c r="F31" s="3"/>
-      <c r="G31" s="3"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="4"/>
+      <c r="G31" s="4"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B32" t="e">
@@ -1588,7 +1600,7 @@
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B33">
         <f>COUNT(D:D)</f>
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D33" t="b">
         <f>C30=D30</f>
@@ -1604,17 +1616,17 @@
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="3" t="s">
+      <c r="A35" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B35" s="3"/>
-      <c r="C35" s="3"/>
-      <c r="D35" s="3"/>
-      <c r="E35" s="3"/>
-      <c r="F35" s="3"/>
-      <c r="G35" s="3"/>
-      <c r="H35" s="3"/>
-      <c r="I35" s="4"/>
+      <c r="B35" s="4"/>
+      <c r="C35" s="4"/>
+      <c r="D35" s="4"/>
+      <c r="E35" s="4"/>
+      <c r="F35" s="4"/>
+      <c r="G35" s="4"/>
+      <c r="H35" s="4"/>
+      <c r="I35" s="5"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">

</xml_diff>

<commit_message>
Fixed bug when calculating single worksheets or ranges
</commit_message>
<xml_diff>
--- a/EPPlusTest/Workbooks/FormulaTest.xlsx
+++ b/EPPlusTest/Workbooks/FormulaTest.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="49">
   <si>
     <t>Functions</t>
   </si>
@@ -177,6 +177,9 @@
   </si>
   <si>
     <t>Boolean</t>
+  </si>
+  <si>
+    <t>If</t>
   </si>
 </sst>
 </file>
@@ -705,10 +708,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:P41"/>
+  <dimension ref="A1:P42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1569,190 +1572,207 @@
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B31" s="1" t="s">
+      <c r="A31" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B31">
+        <f>IF(B2&gt;3,B3,B5)</f>
+        <v>18</v>
+      </c>
+      <c r="C31">
+        <f>IF((B2*B3)*C1&lt;0,(B2*B3)*C1,ABS((B2*B3)*C1))</f>
+        <v>-378.72023092760963</v>
+      </c>
+      <c r="D31">
+        <f>IF((B2*B3)*C1&lt;0,ABS((B2*B3)*C1),(B2*B3)*C1)</f>
+        <v>378.72023092760963</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B32" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D31" s="4" t="s">
+      <c r="D32" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="E31" s="4"/>
-      <c r="F31" s="4"/>
-      <c r="G31" s="4"/>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B32" t="e">
+      <c r="E32" s="4"/>
+      <c r="F32" s="4"/>
+      <c r="G32" s="4"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B33" t="e">
         <f>SUM(D:D)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="D32" t="b">
+      <c r="D33" t="b">
         <f>B4=B3</f>
         <v>0</v>
       </c>
-      <c r="E32" t="b">
+      <c r="E33" t="b">
         <f>C25=D25</f>
         <v>1</v>
       </c>
-      <c r="F32" t="e">
-        <f>E37=E38</f>
+      <c r="F33" t="e">
+        <f>E38=E39</f>
         <v>#N/A</v>
       </c>
-      <c r="G32" t="b">
+      <c r="G33" t="b">
         <f>LEFT(A22,5)=LEFT(A23,5)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B33">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B34">
         <f>COUNT(D:D)</f>
-        <v>23</v>
-      </c>
-      <c r="D33" t="b">
+        <v>24</v>
+      </c>
+      <c r="D34" t="b">
         <f>C30=D30</f>
         <v>1</v>
       </c>
-      <c r="E33" t="e">
-        <f>D37=D38</f>
+      <c r="E34" t="e">
+        <f>D38=D39</f>
         <v>#VALUE!</v>
       </c>
-      <c r="F33" t="e">
-        <f>G37=H37</f>
+      <c r="F34" t="e">
+        <f>G38=H38</f>
         <v>#NULL!</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="4" t="s">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B35" s="4"/>
-      <c r="C35" s="4"/>
-      <c r="D35" s="4"/>
-      <c r="E35" s="4"/>
-      <c r="F35" s="4"/>
-      <c r="G35" s="4"/>
-      <c r="H35" s="4"/>
-      <c r="I35" s="5"/>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
+      <c r="B36" s="4"/>
+      <c r="C36" s="4"/>
+      <c r="D36" s="4"/>
+      <c r="E36" s="4"/>
+      <c r="F36" s="4"/>
+      <c r="G36" s="4"/>
+      <c r="H36" s="4"/>
+      <c r="I36" s="5"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="B37" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="C37" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D36" s="1" t="s">
+      <c r="D37" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E36" s="1" t="s">
+      <c r="E37" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F36" s="1" t="s">
+      <c r="F37" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="G36" s="1" t="s">
+      <c r="G37" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="H36" s="1" t="s">
+      <c r="H37" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I36" s="1" t="s">
+      <c r="I37" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" t="e">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" t="e">
         <f>d</f>
         <v>#NAME?</v>
       </c>
-      <c r="B37" t="e">
-        <f>SUM(I37)</f>
+      <c r="B38" t="e">
+        <f>SUM(I38)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="C37" t="e">
+      <c r="C38" t="e">
         <f>SUM(C2:C3)</f>
         <v>#NAME?</v>
       </c>
-      <c r="D37" t="e">
+      <c r="D38" t="e">
         <f>1+"a"</f>
         <v>#VALUE!</v>
       </c>
-      <c r="E37" t="e">
+      <c r="E38" t="e">
         <f>VLOOKUP(8,I9:I27,0,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="F37" t="e">
+      <c r="F38" t="e">
         <f>POWER(100,10000000000000)</f>
         <v>#NUM!</v>
       </c>
-      <c r="G37" t="e">
+      <c r="G38" t="e">
         <f>B1 B2</f>
         <v>#NULL!</v>
       </c>
-      <c r="H37" t="e">
+      <c r="H38" t="e">
         <f>SUM(#REF!:B3)</f>
         <v>#REF!</v>
       </c>
-      <c r="I37" t="e">
+      <c r="I38" t="e">
         <f>0/0</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" t="e">
-        <f>SUM(A37)</f>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" t="e">
+        <f>SUM(A38)</f>
         <v>#NAME?</v>
       </c>
-      <c r="D38" t="e">
+      <c r="D39" t="e">
         <f>SUBTOTAL(45,J9:J26)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="E38" t="e">
+      <c r="E39" t="e">
         <f>NA()</f>
         <v>#N/A</v>
       </c>
-      <c r="H38" t="e">
+      <c r="H39" t="e">
         <f>MAX(#REF!)</f>
         <v>#REF!</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" t="e">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" t="e">
         <f ca="1">Dp()</f>
         <v>#NAME?</v>
       </c>
-      <c r="D39" t="e">
+      <c r="D40" t="e">
         <f>SUMPRODUCT(B2,B3:B4)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="H39" t="e">
+      <c r="H40" t="e">
         <f>#REF!:#REF!</f>
         <v>#REF!</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40"/>
-      <c r="D40" t="e">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41"/>
+      <c r="D41" t="e">
         <f>B1:B2</f>
         <v>#VALUE!</v>
       </c>
-      <c r="H40" t="e">
+      <c r="H41" t="e">
         <f ca="1">D5()</f>
         <v>#REF!</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41"/>
-      <c r="H41" t="e">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42"/>
+      <c r="H42" t="e">
         <f ca="1">D5(21)</f>
         <v>#REF!</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A35:I35"/>
-    <mergeCell ref="D31:G31"/>
+    <mergeCell ref="A36:I36"/>
+    <mergeCell ref="D32:G32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>